<commit_message>
Slew of new files with data and 2 attempts at writing a different DFT.
</commit_message>
<xml_diff>
--- a/fourier_dataset.xlsx
+++ b/fourier_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astev\Documents\Fourier Transforms\FFT-algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{489E38C0-7394-46C4-95A9-5FD1BE27D70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116BC77E-9280-4A87-9FAD-CE323BDBE841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74AC62C9-4F2A-4A82-A840-8603D2890C1B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Constants</t>
   </si>
@@ -86,58 +86,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>1</t>
     </r>
     <r>
@@ -165,6 +113,58 @@
   </si>
   <si>
     <t>f(t)</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -315,7 +315,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -639,304 +651,304 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7207105049300226</c:v>
+                  <c:v>1.8245847534087343</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.072203391035127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0892647180232871E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.33999725444884044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.56451124273863307</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.2934351331176011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.4176948938476537</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.30204226747136625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8245847534087338</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0722033910351276</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0892647180233093E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.33999725444884049</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.56451124273863307</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.2934351331176008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.4176948938476537</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.30204226747136675</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>1.8245847534087343</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5708756945544053</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.072203391035127</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0892647180232871E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.26185870017945789</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="22">
+                  <c:v>1.0722033910351247</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0892647180235702E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.33999725444884066</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.5645112427386324</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.2934351331176006</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.4176948938476539</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.30204226747136742</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.2499999999999984</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.8245847534087343</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0722033910351283</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.0892647180233759E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>-0.33999725444884044</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.29365952180518057</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="35">
                   <c:v>-0.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.32390825826260261</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.56451124273863307</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.92883617263419893</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.2934351331176011</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-1.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-1.4176948938476537</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.99821481049064353</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.30204226747136625</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.51489126388765438</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.2499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.7207105049300226</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.8245847534087338</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.5708756945544067</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0722033910351276</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.50000000000000044</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.0892647180233093E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-0.26185870017945778</c:v>
-                </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="36">
+                  <c:v>-0.56451124273863229</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.2934351331176002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4176948938476541</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.30204226747136809</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.249999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.8245847534087356</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.072203391035129</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.0892647180233981E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.33999725444884055</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.56451124273862852</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.2934351331175999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.4176948938476543</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.30204226747135976</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.2499999999999976</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.8245847534087356</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.0722033910351292</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.0892647180238755E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-0.33999725444884055</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.56451124273863185</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-1.2934351331176033</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-1.4176948938476543</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.30204226747136043</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2499999999999971</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.8245847534087356</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0722033910351296</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.0892647180239088E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>-0.33999725444884049</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>-0.29365952180518051</c:v>
-                </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="65">
                   <c:v>-0.25</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>-0.32390825826260206</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-0.56451124273863307</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-0.92883617263419893</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-1.2934351331176008</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-1.4999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-1.4176948938476537</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-0.99821481049064387</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-0.30204226747136675</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.51489126388765361</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.2499999999999991</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.7207105049300206</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.8245847534087343</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.570875694554406</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.0722033910351247</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.50000000000000089</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2.0892647180235702E-2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-0.26185870017945756</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-0.33999725444884066</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-0.2936595218051804</c:v>
-                </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="66">
+                  <c:v>-0.56451124273863151</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.2934351331176033</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.4176948938476546</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.30204226747136087</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.2499999999999967</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.8245847534087358</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.0722033910351303</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.089264718023931E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.33999725444884044</c:v>
+                </c:pt>
+                <c:pt idx="75">
                   <c:v>-0.25</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>-0.32390825826260111</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-0.5645112427386324</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-0.92883617263419638</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-1.2934351331176006</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-1.4999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-1.4176948938476539</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-0.99821481049064109</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-0.30204226747136742</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.51489126388765771</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.2499999999999984</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1.7207105049300204</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.8245847534087343</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1.5708756945544085</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.0722033910351283</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.49999999999999822</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2.0892647180233759E-2</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>-0.26185870017945845</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>-0.33999725444884044</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-0.2936595218051804</c:v>
-                </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="76">
+                  <c:v>-0.5645112427386314</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-1.2934351331176031</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-1.4176948938476548</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.30204226747136154</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.8245847534087358</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.0722033910351434</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.0892647180230761E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.33999725444884055</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>-0.25</c:v>
                 </c:pt>
-                <c:pt idx="71">
-                  <c:v>-0.32390825826260095</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>-0.56451124273863229</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-0.92883617263419604</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>-1.2934351331176002</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>-1.4999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>-1.4176948938476541</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>-0.99821481049064154</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>-0.30204226747136809</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.51489126388765705</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.249999999999998</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1.7207105049300202</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1.8245847534087356</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1.5708756945544045</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.072203391035129</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.49999999999999867</c:v>
-                </c:pt>
                 <c:pt idx="86">
-                  <c:v>2.0892647180233981E-2</c:v>
+                  <c:v>-0.56451124273863096</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-0.26185870017945634</c:v>
+                  <c:v>-1.2934351331175957</c:v>
                 </c:pt>
                 <c:pt idx="88">
+                  <c:v>-1.4176948938476495</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.3020422674713622</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.2499999999999956</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.8245847534087358</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.0722033910351441</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.0892647180231205E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
                   <c:v>-0.33999725444884055</c:v>
                 </c:pt>
-                <c:pt idx="89">
-                  <c:v>-0.29365952180518046</c:v>
-                </c:pt>
-                <c:pt idx="90">
+                <c:pt idx="95">
                   <c:v>-0.25</c:v>
                 </c:pt>
-                <c:pt idx="91">
-                  <c:v>-0.32390825826260083</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>-0.56451124273862852</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>-0.92883617263419993</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>-1.2934351331175999</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>-1.4999999999999993</c:v>
-                </c:pt>
                 <c:pt idx="96">
-                  <c:v>-1.4176948938476543</c:v>
+                  <c:v>-0.56451124273863085</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>-0.99821481049064842</c:v>
+                  <c:v>-1.2934351331175955</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>-0.30204226747135976</c:v>
+                  <c:v>-1.4176948938476497</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.51489126388765638</c:v>
+                  <c:v>-0.30204226747136287</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.2499999999999976</c:v>
+                  <c:v>1.2499999999999951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77E55F4-C1DD-4659-A826-6C251FB08CAD}">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2068,19 +2080,22 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.35">
@@ -2094,20 +2109,23 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>B$3*SIN(B$2*PI()*D2)</f>
+        <f>B$3*SIN(B$2*2*PI()*D2)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>B$4*COS(B$2*PI()*D2)</f>
+        <f>B$4*COS(B$2*2*PI()*D2)</f>
         <v>0.75</v>
       </c>
       <c r="G2">
-        <f>B$5*SIN(2*B$2*PI()*D2)</f>
+        <f>B$5*SIN(2*B$2*2*PI()*D2)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>B$5*COS(2*B$2*PI()*D2)</f>
+        <f>B$5*COS(2*B$2*2*PI()*D2)</f>
         <v>0.5</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
       </c>
       <c r="N2">
         <f>SUM(E2,F2,G2,H2)</f>
@@ -2125,29 +2143,32 @@
         <v>0.1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">B$3*SIN(B$2*PI()*D3)</f>
-        <v>0.3090169943749474</v>
+        <f t="shared" ref="E3:E66" si="0">B$3*SIN(B$2*2*PI()*D3)</f>
+        <v>0.58778525229247314</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="1">B$4*COS(B$2*PI()*D3)</f>
-        <v>0.71329238722136512</v>
+        <f t="shared" ref="F3:F66" si="1">B$4*COS(B$2*2*PI()*D3)</f>
+        <v>0.60676274578121059</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="2">B$5*SIN(2*B$2*PI()*D3)</f>
-        <v>0.29389262614623657</v>
+        <f t="shared" ref="G3:G66" si="2">B$5*SIN(2*B$2*2*PI()*D3)</f>
+        <v>0.47552825814757677</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="3">B$5*COS(2*B$2*PI()*D3)</f>
-        <v>0.40450849718747373</v>
+        <f t="shared" ref="H3:H66" si="3">B$5*COS(2*B$2*2*PI()*D3)</f>
+        <v>0.15450849718747373</v>
+      </c>
+      <c r="M3">
+        <v>0.1</v>
       </c>
       <c r="N3">
         <f>SUM(E3,F3,G3,H3)</f>
-        <v>1.7207105049300226</v>
+        <v>1.8245847534087343</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0.75</v>
@@ -2157,28 +2178,31 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.58778525229247314</v>
+        <v>0.95105651629515353</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>0.60676274578121059</v>
+        <v>0.23176274578121059</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>0.47552825814757677</v>
+        <v>0.29389262614623662</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>0.15450849718747373</v>
+        <v>-0.40450849718747367</v>
+      </c>
+      <c r="M4">
+        <v>0.2</v>
       </c>
       <c r="N4">
         <f>SUM(E4,F4,G4,H4)</f>
-        <v>1.8245847534087343</v>
+        <v>1.072203391035127</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -2188,23 +2212,26 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.80901699437494745</v>
+        <v>0.95105651629515364</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>0.44083893921935485</v>
+        <v>-0.23176274578121051</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0.47552825814757682</v>
+        <v>-0.29389262614623651</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747367</v>
+        <v>-0.40450849718747378</v>
+      </c>
+      <c r="M5">
+        <v>0.3</v>
       </c>
       <c r="N5">
         <f>SUM(E5,F5,G5,H5)</f>
-        <v>1.5708756945544053</v>
+        <v>2.0892647180232871E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -2213,23 +2240,26 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.95105651629515353</v>
+        <v>0.58778525229247325</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>0.23176274578121059</v>
+        <v>-0.60676274578121048</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>0.29389262614623662</v>
+        <v>-0.47552825814757682</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747367</v>
+        <v>0.15450849718747361</v>
+      </c>
+      <c r="M6">
+        <v>0.4</v>
       </c>
       <c r="N6">
         <f>SUM(E6,F6,G6,H6)</f>
-        <v>1.072203391035127</v>
+        <v>-0.33999725444884044</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -2238,23 +2268,26 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>4.594306705907325E-17</v>
+        <v>-0.75</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>6.1257422745431001E-17</v>
+        <v>-1.22514845490862E-16</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M7">
+        <v>0.5</v>
       </c>
       <c r="N7">
         <f>SUM(E7,F7,G7,H7)</f>
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2263,23 +2296,26 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.95105651629515364</v>
+        <v>-0.58778525229247303</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>-0.23176274578121051</v>
+        <v>-0.6067627457812107</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623651</v>
+        <v>0.47552825814757677</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747378</v>
+        <v>0.15450849718747386</v>
+      </c>
+      <c r="M8">
+        <v>0.6</v>
       </c>
       <c r="N8">
         <f>SUM(E8,F8,G8,H8)</f>
-        <v>2.0892647180232871E-2</v>
+        <v>-0.56451124273863307</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -2288,23 +2324,26 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.80901699437494745</v>
+        <v>-0.95105651629515353</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>-0.4408389392193548</v>
+        <v>-0.23176274578121067</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757677</v>
+        <v>0.29389262614623668</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747378</v>
+        <v>-0.40450849718747361</v>
+      </c>
+      <c r="M9">
+        <v>0.7</v>
       </c>
       <c r="N9">
         <f>SUM(E9,F9,G9,H9)</f>
-        <v>-0.26185870017945789</v>
+        <v>-1.2934351331176011</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -2313,23 +2352,26 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0.58778525229247325</v>
+        <v>-0.95105651629515364</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>-0.60676274578121048</v>
+        <v>0.23176274578121042</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757682</v>
+        <v>-0.2938926261462364</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>0.15450849718747361</v>
+        <v>-0.40450849718747384</v>
+      </c>
+      <c r="M10">
+        <v>0.8</v>
       </c>
       <c r="N10">
         <f>SUM(E10,F10,G10,H10)</f>
-        <v>-0.33999725444884044</v>
+        <v>-1.4176948938476537</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -2338,23 +2380,26 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0.30901699437494751</v>
+        <v>-0.58778525229247336</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136512</v>
+        <v>0.60676274578121048</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623668</v>
+        <v>-0.47552825814757688</v>
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>0.40450849718747367</v>
+        <v>0.1545084971874735</v>
+      </c>
+      <c r="M11">
+        <v>0.9</v>
       </c>
       <c r="N11">
         <f>SUM(E11,F11,G11,H11)</f>
-        <v>-0.29365952180518057</v>
+        <v>-0.30204226747136625</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -2363,23 +2408,26 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1.22514845490862E-16</v>
+        <v>-2.45029690981724E-16</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>-1.22514845490862E-16</v>
+        <v>-2.45029690981724E-16</v>
       </c>
       <c r="H12">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
       </c>
       <c r="N12">
         <f>SUM(E12,F12,G12,H12)</f>
-        <v>-0.25</v>
+        <v>1.2499999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -2388,23 +2436,26 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>-0.30901699437494773</v>
+        <v>0.58778525229247358</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136512</v>
+        <v>0.60676274578121026</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>0.29389262614623679</v>
+        <v>0.47552825814757699</v>
       </c>
       <c r="H13">
         <f t="shared" si="3"/>
-        <v>0.4045084971874735</v>
+        <v>0.15450849718747312</v>
+      </c>
+      <c r="M13">
+        <v>1.1000000000000001</v>
       </c>
       <c r="N13">
         <f>SUM(E13,F13,G13,H13)</f>
-        <v>-0.32390825826260261</v>
+        <v>1.8245847534087338</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -2413,23 +2464,26 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-0.58778525229247303</v>
+        <v>0.95105651629515353</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>-0.6067627457812107</v>
+        <v>0.23176274578121081</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0.47552825814757677</v>
+        <v>0.29389262614623679</v>
       </c>
       <c r="H14">
         <f t="shared" si="3"/>
-        <v>0.15450849718747386</v>
+        <v>-0.40450849718747356</v>
+      </c>
+      <c r="M14">
+        <v>1.2</v>
       </c>
       <c r="N14">
         <f>SUM(E14,F14,G14,H14)</f>
-        <v>-0.56451124273863307</v>
+        <v>1.0722033910351276</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -2438,23 +2492,26 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494734</v>
+        <v>0.95105651629515364</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>-0.44083893921935491</v>
+        <v>-0.23176274578121034</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>0.47552825814757682</v>
+        <v>-0.29389262614623629</v>
       </c>
       <c r="H15">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747356</v>
+        <v>-0.40450849718747389</v>
+      </c>
+      <c r="M15">
+        <v>1.3</v>
       </c>
       <c r="N15">
         <f>SUM(E15,F15,G15,H15)</f>
-        <v>-0.92883617263419893</v>
+        <v>2.0892647180233093E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -2463,23 +2520,26 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515353</v>
+        <v>0.58778525229247336</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>-0.23176274578121067</v>
+        <v>-0.60676274578121037</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>0.29389262614623668</v>
+        <v>-0.47552825814757688</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747361</v>
+        <v>0.15450849718747339</v>
+      </c>
+      <c r="M16">
+        <v>1.4</v>
       </c>
       <c r="N16">
         <f>SUM(E16,F16,G16,H16)</f>
-        <v>-1.2934351331176011</v>
+        <v>-0.33999725444884049</v>
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.3">
@@ -2488,23 +2548,26 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>-1.3782920117721975E-16</v>
+        <v>-0.75</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>1.83772268236293E-16</v>
+        <v>-3.67544536472586E-16</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M17">
+        <v>1.5</v>
       </c>
       <c r="N17">
         <f>SUM(E17,F17,G17,H17)</f>
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.3">
@@ -2513,23 +2576,26 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515364</v>
+        <v>-0.5877852522924728</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0.23176274578121042</v>
+        <v>-0.60676274578121081</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>-0.2938926261462364</v>
+        <v>0.47552825814757665</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747384</v>
+        <v>0.15450849718747409</v>
+      </c>
+      <c r="M18">
+        <v>1.6</v>
       </c>
       <c r="N18">
         <f>SUM(E18,F18,G18,H18)</f>
-        <v>-1.4176948938476537</v>
+        <v>-0.56451124273863307</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.3">
@@ -2538,23 +2604,26 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494756</v>
+        <v>-0.95105651629515342</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0.44083893921935469</v>
+        <v>-0.23176274578121087</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757671</v>
+        <v>0.2938926261462369</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747392</v>
+        <v>-0.40450849718747345</v>
+      </c>
+      <c r="M19">
+        <v>1.7</v>
       </c>
       <c r="N19">
         <f>SUM(E19,F19,G19,H19)</f>
-        <v>-0.99821481049064353</v>
+        <v>-1.2934351331176008</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.3">
@@ -2563,23 +2632,26 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-0.58778525229247336</v>
+        <v>-0.95105651629515375</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>0.60676274578121048</v>
+        <v>0.23176274578121026</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757688</v>
+        <v>-0.29389262614623624</v>
       </c>
       <c r="H20">
         <f t="shared" si="3"/>
-        <v>0.1545084971874735</v>
+        <v>-0.40450849718747395</v>
+      </c>
+      <c r="M20">
+        <v>1.8</v>
       </c>
       <c r="N20">
         <f>SUM(E20,F20,G20,H20)</f>
-        <v>-0.30204226747136625</v>
+        <v>-1.4176948938476537</v>
       </c>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.3">
@@ -2588,23 +2660,26 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>-0.30901699437494762</v>
+        <v>-0.58778525229247347</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>0.71329238722136512</v>
+        <v>0.60676274578121037</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623674</v>
+        <v>-0.47552825814757693</v>
       </c>
       <c r="H21">
         <f t="shared" si="3"/>
-        <v>0.40450849718747356</v>
+        <v>0.15450849718747328</v>
+      </c>
+      <c r="M21">
+        <v>1.9</v>
       </c>
       <c r="N21">
         <f>SUM(E21,F21,G21,H21)</f>
-        <v>0.51489126388765438</v>
+        <v>-0.30204226747136675</v>
       </c>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.3">
@@ -2613,7 +2688,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>-2.45029690981724E-16</v>
+        <v>-4.90059381963448E-16</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
@@ -2621,15 +2696,18 @@
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>-2.45029690981724E-16</v>
+        <v>-4.90059381963448E-16</v>
       </c>
       <c r="H22">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
       </c>
       <c r="N22">
         <f>SUM(E22,F22,G22,H22)</f>
-        <v>1.2499999999999996</v>
+        <v>1.2499999999999991</v>
       </c>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.3">
@@ -2638,23 +2716,26 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0.30901699437494717</v>
+        <v>0.58778525229247269</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>0.71329238722136523</v>
+        <v>0.60676274578121081</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>0.29389262614623635</v>
+        <v>0.47552825814757665</v>
       </c>
       <c r="H23">
         <f t="shared" si="3"/>
-        <v>0.40450849718747384</v>
+        <v>0.1545084971874742</v>
+      </c>
+      <c r="M23">
+        <v>2.1</v>
       </c>
       <c r="N23">
         <f>SUM(E23,F23,G23,H23)</f>
-        <v>1.7207105049300226</v>
+        <v>1.8245847534087343</v>
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.3">
@@ -2663,23 +2744,26 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>0.58778525229247358</v>
+        <v>0.95105651629515398</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0.60676274578121026</v>
+        <v>0.23176274578120967</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>0.47552825814757699</v>
+        <v>0.29389262614623557</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
-        <v>0.15450849718747312</v>
+        <v>-0.40450849718747445</v>
+      </c>
+      <c r="M24">
+        <v>2.2000000000000002</v>
       </c>
       <c r="N24">
         <f>SUM(E24,F24,G24,H24)</f>
-        <v>1.8245847534087338</v>
+        <v>1.0722033910351247</v>
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.3">
@@ -2688,23 +2772,26 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>0.80901699437494679</v>
+        <v>0.95105651629515431</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0.44083893921935552</v>
+        <v>-0.23176274578120887</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>0.47552825814757715</v>
+        <v>-0.29389262614623468</v>
       </c>
       <c r="H25">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747259</v>
+        <v>-0.40450849718747511</v>
+      </c>
+      <c r="M25">
+        <v>2.2999999999999998</v>
       </c>
       <c r="N25">
         <f>SUM(E25,F25,G25,H25)</f>
-        <v>1.5708756945544067</v>
+        <v>2.0892647180235702E-2</v>
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.3">
@@ -2713,23 +2800,26 @@
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>0.95105651629515353</v>
+        <v>0.58778525229247358</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>0.23176274578121081</v>
+        <v>-0.60676274578121037</v>
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>0.29389262614623679</v>
+        <v>-0.47552825814757699</v>
       </c>
       <c r="H26">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747356</v>
+        <v>0.15450849718747314</v>
+      </c>
+      <c r="M26">
+        <v>2.4</v>
       </c>
       <c r="N26">
         <f>SUM(E26,F26,G26,H26)</f>
-        <v>1.0722033910351276</v>
+        <v>-0.33999725444884066</v>
       </c>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.3">
@@ -2738,23 +2828,26 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6.1257422745431001E-16</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>2.2971533529536625E-16</v>
+        <v>-0.75</v>
       </c>
       <c r="G27">
         <f t="shared" si="2"/>
-        <v>3.06287113727155E-16</v>
+        <v>-6.1257422745431001E-16</v>
       </c>
       <c r="H27">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M27">
+        <v>2.5</v>
       </c>
       <c r="N27">
         <f>SUM(E27,F27,G27,H27)</f>
-        <v>0.50000000000000044</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.3">
@@ -2763,23 +2856,26 @@
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>0.95105651629515364</v>
+        <v>-0.58778525229247258</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>-0.23176274578121034</v>
+        <v>-0.60676274578121081</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623629</v>
+        <v>0.4755282581475766</v>
       </c>
       <c r="H28">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747389</v>
+        <v>0.15450849718747431</v>
+      </c>
+      <c r="M28">
+        <v>2.6</v>
       </c>
       <c r="N28">
         <f>SUM(E28,F28,G28,H28)</f>
-        <v>2.0892647180233093E-2</v>
+        <v>-0.5645112427386324</v>
       </c>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.3">
@@ -2788,23 +2884,26 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>0.80901699437494767</v>
+        <v>-0.95105651629515342</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>-0.44083893921935469</v>
+        <v>-0.23176274578121103</v>
       </c>
       <c r="G29">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757671</v>
+        <v>0.29389262614623712</v>
       </c>
       <c r="H29">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747403</v>
+        <v>-0.40450849718747334</v>
+      </c>
+      <c r="M29">
+        <v>2.7</v>
       </c>
       <c r="N29">
         <f>SUM(E29,F29,G29,H29)</f>
-        <v>-0.26185870017945778</v>
+        <v>-1.2934351331176006</v>
       </c>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.3">
@@ -2813,23 +2912,26 @@
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>0.58778525229247336</v>
+        <v>-0.95105651629515375</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>-0.60676274578121037</v>
+        <v>0.23176274578121009</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757688</v>
+        <v>-0.29389262614623601</v>
       </c>
       <c r="H30">
         <f t="shared" si="3"/>
-        <v>0.15450849718747339</v>
+        <v>-0.40450849718747411</v>
+      </c>
+      <c r="M30">
+        <v>2.8</v>
       </c>
       <c r="N30">
         <f>SUM(E30,F30,G30,H30)</f>
-        <v>-0.33999725444884049</v>
+        <v>-1.4176948938476539</v>
       </c>
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.3">
@@ -2838,23 +2940,26 @@
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>0.30901699437494778</v>
+        <v>-0.58778525229247369</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136501</v>
+        <v>0.60676274578121026</v>
       </c>
       <c r="G31">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623685</v>
+        <v>-0.47552825814757699</v>
       </c>
       <c r="H31">
         <f t="shared" si="3"/>
-        <v>0.4045084971874735</v>
+        <v>0.15450849718747303</v>
+      </c>
+      <c r="M31">
+        <v>2.9</v>
       </c>
       <c r="N31">
         <f>SUM(E31,F31,G31,H31)</f>
-        <v>-0.29365952180518051</v>
+        <v>-0.30204226747136742</v>
       </c>
     </row>
     <row r="32" spans="4:14" x14ac:dyDescent="0.3">
@@ -2863,23 +2968,26 @@
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>3.67544536472586E-16</v>
+        <v>-7.3508907294517201E-16</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G32">
         <f t="shared" si="2"/>
-        <v>-3.67544536472586E-16</v>
+        <v>-7.3508907294517201E-16</v>
       </c>
       <c r="H32">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
       </c>
       <c r="N32">
         <f>SUM(E32,F32,G32,H32)</f>
-        <v>-0.25</v>
+        <v>1.2499999999999984</v>
       </c>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.3">
@@ -2888,23 +2996,26 @@
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>-0.30901699437494706</v>
+        <v>0.58778525229247247</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136523</v>
+        <v>0.60676274578121092</v>
       </c>
       <c r="G33">
         <f t="shared" si="2"/>
-        <v>0.29389262614623624</v>
+        <v>0.47552825814757654</v>
       </c>
       <c r="H33">
         <f t="shared" si="3"/>
-        <v>0.40450849718747395</v>
+        <v>0.15450849718747445</v>
+      </c>
+      <c r="M33">
+        <v>3.1</v>
       </c>
       <c r="N33">
         <f>SUM(E33,F33,G33,H33)</f>
-        <v>-0.32390825826260206</v>
+        <v>1.8245847534087343</v>
       </c>
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.3">
@@ -2913,23 +3024,26 @@
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>-0.5877852522924728</v>
+        <v>0.95105651629515331</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>-0.60676274578121081</v>
+        <v>0.23176274578121114</v>
       </c>
       <c r="G34">
         <f t="shared" si="2"/>
-        <v>0.47552825814757665</v>
+        <v>0.29389262614623718</v>
       </c>
       <c r="H34">
         <f t="shared" si="3"/>
-        <v>0.15450849718747409</v>
+        <v>-0.40450849718747323</v>
+      </c>
+      <c r="M34">
+        <v>3.2</v>
       </c>
       <c r="N34">
         <f>SUM(E34,F34,G34,H34)</f>
-        <v>-0.56451124273863307</v>
+        <v>1.0722033910351283</v>
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.3">
@@ -2938,23 +3052,26 @@
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494723</v>
+        <v>0.95105651629515386</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>-0.44083893921935513</v>
+        <v>-0.23176274578121001</v>
       </c>
       <c r="G35">
         <f t="shared" si="2"/>
-        <v>0.47552825814757693</v>
+        <v>-0.2938926261462359</v>
       </c>
       <c r="H35">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747334</v>
+        <v>-0.40450849718747417</v>
+      </c>
+      <c r="M35">
+        <v>3.3</v>
       </c>
       <c r="N35">
         <f>SUM(E35,F35,G35,H35)</f>
-        <v>-0.92883617263419893</v>
+        <v>2.0892647180233759E-2</v>
       </c>
     </row>
     <row r="36" spans="4:14" x14ac:dyDescent="0.3">
@@ -2963,23 +3080,26 @@
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515342</v>
+        <v>0.5877852522924738</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>-0.23176274578121087</v>
+        <v>-0.60676274578121014</v>
       </c>
       <c r="G36">
         <f t="shared" si="2"/>
-        <v>0.2938926261462369</v>
+        <v>-0.47552825814757704</v>
       </c>
       <c r="H36">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747345</v>
+        <v>0.15450849718747292</v>
+      </c>
+      <c r="M36">
+        <v>3.4</v>
       </c>
       <c r="N36">
         <f>SUM(E36,F36,G36,H36)</f>
-        <v>-1.2934351331176008</v>
+        <v>-0.33999725444884044</v>
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.3">
@@ -2988,23 +3108,26 @@
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>8.5760391843603401E-16</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>-3.2160146941351275E-16</v>
+        <v>-0.75</v>
       </c>
       <c r="G37">
         <f t="shared" si="2"/>
-        <v>4.28801959218017E-16</v>
+        <v>-8.5760391843603401E-16</v>
       </c>
       <c r="H37">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M37">
+        <v>3.5</v>
       </c>
       <c r="N37">
         <f>SUM(E37,F37,G37,H37)</f>
-        <v>-1.4999999999999998</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="38" spans="4:14" x14ac:dyDescent="0.3">
@@ -3013,23 +3136,26 @@
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515375</v>
+        <v>-0.58778525229247247</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>0.23176274578121026</v>
+        <v>-0.60676274578121092</v>
       </c>
       <c r="G38">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623624</v>
+        <v>0.47552825814757649</v>
       </c>
       <c r="H38">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747395</v>
+        <v>0.15450849718747456</v>
+      </c>
+      <c r="M38">
+        <v>3.6</v>
       </c>
       <c r="N38">
         <f>SUM(E38,F38,G38,H38)</f>
-        <v>-1.4176948938476537</v>
+        <v>-0.56451124273863229</v>
       </c>
     </row>
     <row r="39" spans="4:14" x14ac:dyDescent="0.3">
@@ -3038,23 +3164,26 @@
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494767</v>
+        <v>-0.95105651629515331</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>0.44083893921935458</v>
+        <v>-0.2317627457812112</v>
       </c>
       <c r="G39">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757665</v>
+        <v>0.29389262614623729</v>
       </c>
       <c r="H39">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747414</v>
+        <v>-0.40450849718747317</v>
+      </c>
+      <c r="M39">
+        <v>3.7</v>
       </c>
       <c r="N39">
         <f>SUM(E39,F39,G39,H39)</f>
-        <v>-0.99821481049064387</v>
+        <v>-1.2934351331176002</v>
       </c>
     </row>
     <row r="40" spans="4:14" x14ac:dyDescent="0.3">
@@ -3063,23 +3192,26 @@
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>-0.58778525229247347</v>
+        <v>-0.95105651629515386</v>
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>0.60676274578121037</v>
+        <v>0.23176274578120992</v>
       </c>
       <c r="G40">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757693</v>
+        <v>-0.29389262614623579</v>
       </c>
       <c r="H40">
         <f t="shared" si="3"/>
-        <v>0.15450849718747328</v>
+        <v>-0.40450849718747428</v>
+      </c>
+      <c r="M40">
+        <v>3.8</v>
       </c>
       <c r="N40">
         <f>SUM(E40,F40,G40,H40)</f>
-        <v>-0.30204226747136675</v>
+        <v>-1.4176948938476541</v>
       </c>
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.3">
@@ -3088,23 +3220,26 @@
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>-0.3090169943749479</v>
+        <v>-0.58778525229247391</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>0.71329238722136501</v>
+        <v>0.60676274578121014</v>
       </c>
       <c r="G41">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623696</v>
+        <v>-0.4755282581475771</v>
       </c>
       <c r="H41">
         <f t="shared" si="3"/>
-        <v>0.40450849718747345</v>
+        <v>0.15450849718747281</v>
+      </c>
+      <c r="M41">
+        <v>3.9</v>
       </c>
       <c r="N41">
         <f>SUM(E41,F41,G41,H41)</f>
-        <v>0.51489126388765361</v>
+        <v>-0.30204226747136809</v>
       </c>
     </row>
     <row r="42" spans="4:14" x14ac:dyDescent="0.3">
@@ -3113,7 +3248,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>-4.90059381963448E-16</v>
+        <v>-9.8011876392689601E-16</v>
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
@@ -3121,15 +3256,18 @@
       </c>
       <c r="G42">
         <f t="shared" si="2"/>
-        <v>-4.90059381963448E-16</v>
+        <v>-9.8011876392689601E-16</v>
       </c>
       <c r="H42">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M42">
+        <v>4</v>
       </c>
       <c r="N42">
         <f>SUM(E42,F42,G42,H42)</f>
-        <v>1.2499999999999991</v>
+        <v>1.249999999999998</v>
       </c>
     </row>
     <row r="43" spans="4:14" x14ac:dyDescent="0.3">
@@ -3138,23 +3276,26 @@
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>0.30901699437494523</v>
+        <v>0.58778525229246947</v>
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>0.71329238722136568</v>
+        <v>0.60676274578121259</v>
       </c>
       <c r="G43">
         <f t="shared" si="2"/>
-        <v>0.29389262614623474</v>
+        <v>0.47552825814757538</v>
       </c>
       <c r="H43">
         <f t="shared" si="3"/>
-        <v>0.40450849718747506</v>
+        <v>0.15450849718747806</v>
+      </c>
+      <c r="M43">
+        <v>4.0999999999999996</v>
       </c>
       <c r="N43">
         <f>SUM(E43,F43,G43,H43)</f>
-        <v>1.7207105049300206</v>
+        <v>1.8245847534087356</v>
       </c>
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.3">
@@ -3163,23 +3304,26 @@
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
-        <v>0.58778525229247269</v>
+        <v>0.95105651629515331</v>
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>0.60676274578121081</v>
+        <v>0.23176274578121131</v>
       </c>
       <c r="G44">
         <f t="shared" si="2"/>
-        <v>0.47552825814757665</v>
+        <v>0.2938926261462374</v>
       </c>
       <c r="H44">
         <f t="shared" si="3"/>
-        <v>0.1545084971874742</v>
+        <v>-0.40450849718747312</v>
+      </c>
+      <c r="M44">
+        <v>4.2</v>
       </c>
       <c r="N44">
         <f>SUM(E44,F44,G44,H44)</f>
-        <v>1.8245847534087343</v>
+        <v>1.072203391035129</v>
       </c>
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.3">
@@ -3188,23 +3332,26 @@
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
-        <v>0.80901699437494712</v>
+        <v>0.95105651629515386</v>
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>0.44083893921935519</v>
+        <v>-0.23176274578120981</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
-        <v>0.47552825814757693</v>
+        <v>-0.29389262614623574</v>
       </c>
       <c r="H45">
         <f t="shared" si="3"/>
-        <v>-0.1545084971874732</v>
+        <v>-0.40450849718747434</v>
+      </c>
+      <c r="M45">
+        <v>4.3</v>
       </c>
       <c r="N45">
         <f>SUM(E45,F45,G45,H45)</f>
-        <v>1.570875694554406</v>
+        <v>2.0892647180233981E-2</v>
       </c>
     </row>
     <row r="46" spans="4:14" x14ac:dyDescent="0.3">
@@ -3213,23 +3360,26 @@
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
-        <v>0.95105651629515398</v>
+        <v>0.58778525229247114</v>
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>0.23176274578120967</v>
+        <v>-0.6067627457812117</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
-        <v>0.29389262614623557</v>
+        <v>-0.47552825814757604</v>
       </c>
       <c r="H46">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747445</v>
+        <v>0.15450849718747606</v>
+      </c>
+      <c r="M46">
+        <v>4.4000000000000004</v>
       </c>
       <c r="N46">
         <f>SUM(E46,F46,G46,H46)</f>
-        <v>1.0722033910351247</v>
+        <v>-0.33999725444884055</v>
       </c>
     </row>
     <row r="47" spans="4:14" x14ac:dyDescent="0.3">
@@ -3238,23 +3388,26 @@
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.102633609417758E-15</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>4.1348760353165925E-16</v>
+        <v>-0.75</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
-        <v>5.51316804708879E-16</v>
+        <v>-1.102633609417758E-15</v>
       </c>
       <c r="H47">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M47">
+        <v>4.5</v>
       </c>
       <c r="N47">
         <f>SUM(E47,F47,G47,H47)</f>
-        <v>0.50000000000000089</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="48" spans="4:14" x14ac:dyDescent="0.3">
@@ -3263,23 +3416,26 @@
       </c>
       <c r="E48">
         <f t="shared" si="0"/>
-        <v>0.95105651629515431</v>
+        <v>-0.58778525229246936</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>-0.23176274578120887</v>
+        <v>-0.6067627457812127</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623468</v>
+        <v>0.47552825814757532</v>
       </c>
       <c r="H48">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747511</v>
+        <v>0.15450849718747817</v>
+      </c>
+      <c r="M48">
+        <v>4.5999999999999996</v>
       </c>
       <c r="N48">
         <f>SUM(E48,F48,G48,H48)</f>
-        <v>2.0892647180235702E-2</v>
+        <v>-0.56451124273862852</v>
       </c>
     </row>
     <row r="49" spans="4:14" x14ac:dyDescent="0.3">
@@ -3288,23 +3444,26 @@
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>0.80901699437494778</v>
+        <v>-0.9510565162951532</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>-0.44083893921935452</v>
+        <v>-0.23176274578121137</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
-        <v>-0.4755282581475766</v>
+        <v>0.29389262614623751</v>
       </c>
       <c r="H49">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747425</v>
+        <v>-0.40450849718747306</v>
+      </c>
+      <c r="M49">
+        <v>4.7</v>
       </c>
       <c r="N49">
         <f>SUM(E49,F49,G49,H49)</f>
-        <v>-0.26185870017945756</v>
+        <v>-1.2934351331175999</v>
       </c>
     </row>
     <row r="50" spans="4:14" x14ac:dyDescent="0.3">
@@ -3313,23 +3472,26 @@
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>0.58778525229247358</v>
+        <v>-0.95105651629515398</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>-0.60676274578121037</v>
+        <v>0.2317627457812097</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757699</v>
+        <v>-0.29389262614623562</v>
       </c>
       <c r="H50">
         <f t="shared" si="3"/>
-        <v>0.15450849718747314</v>
+        <v>-0.40450849718747439</v>
+      </c>
+      <c r="M50">
+        <v>4.8</v>
       </c>
       <c r="N50">
         <f>SUM(E50,F50,G50,H50)</f>
-        <v>-0.33999725444884066</v>
+        <v>-1.4176948938476543</v>
       </c>
     </row>
     <row r="51" spans="4:14" x14ac:dyDescent="0.3">
@@ -3338,23 +3500,26 @@
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>0.30901699437494629</v>
+        <v>-0.58778525229247125</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136545</v>
+        <v>0.60676274578121159</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623562</v>
+        <v>-0.47552825814757604</v>
       </c>
       <c r="H51">
         <f t="shared" si="3"/>
-        <v>0.40450849718747439</v>
+        <v>0.15450849718747595</v>
+      </c>
+      <c r="M51">
+        <v>4.9000000000000004</v>
       </c>
       <c r="N51">
         <f>SUM(E51,F51,G51,H51)</f>
-        <v>-0.2936595218051804</v>
+        <v>-0.30204226747135976</v>
       </c>
     </row>
     <row r="52" spans="4:14" x14ac:dyDescent="0.3">
@@ -3363,23 +3528,26 @@
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>6.1257422745431001E-16</v>
+        <v>-1.22514845490862E-15</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>-6.1257422745431001E-16</v>
+        <v>-1.22514845490862E-15</v>
       </c>
       <c r="H52">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M52">
+        <v>5</v>
       </c>
       <c r="N52">
         <f>SUM(E52,F52,G52,H52)</f>
-        <v>-0.25</v>
+        <v>1.2499999999999976</v>
       </c>
     </row>
     <row r="53" spans="4:14" x14ac:dyDescent="0.3">
@@ -3388,23 +3556,26 @@
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>-0.30901699437494512</v>
+        <v>0.58778525229246925</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>-0.71329238722136568</v>
+        <v>0.6067627457812127</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
-        <v>0.29389262614623463</v>
+        <v>0.47552825814757532</v>
       </c>
       <c r="H53">
         <f t="shared" si="3"/>
-        <v>0.40450849718747511</v>
+        <v>0.15450849718747828</v>
+      </c>
+      <c r="M53">
+        <v>5.0999999999999996</v>
       </c>
       <c r="N53">
         <f>SUM(E53,F53,G53,H53)</f>
-        <v>-0.32390825826260111</v>
+        <v>1.8245847534087356</v>
       </c>
     </row>
     <row r="54" spans="4:14" x14ac:dyDescent="0.3">
@@ -3413,23 +3584,26 @@
       </c>
       <c r="E54">
         <f t="shared" si="0"/>
-        <v>-0.58778525229247258</v>
+        <v>0.9510565162951532</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
-        <v>-0.60676274578121081</v>
+        <v>0.23176274578121148</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
-        <v>0.4755282581475766</v>
+        <v>0.29389262614623757</v>
       </c>
       <c r="H54">
         <f t="shared" si="3"/>
-        <v>0.15450849718747431</v>
+        <v>-0.40450849718747295</v>
+      </c>
+      <c r="M54">
+        <v>5.2</v>
       </c>
       <c r="N54">
         <f>SUM(E54,F54,G54,H54)</f>
-        <v>-0.5645112427386324</v>
+        <v>1.0722033910351292</v>
       </c>
     </row>
     <row r="55" spans="4:14" x14ac:dyDescent="0.3">
@@ -3438,23 +3612,26 @@
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494601</v>
+        <v>0.95105651629515509</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>-0.44083893921935635</v>
+        <v>-0.23176274578120709</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
-        <v>0.47552825814757754</v>
+        <v>-0.29389262614623263</v>
       </c>
       <c r="H55">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747139</v>
+        <v>-0.40450849718747656</v>
+      </c>
+      <c r="M55">
+        <v>5.3</v>
       </c>
       <c r="N55">
         <f>SUM(E55,F55,G55,H55)</f>
-        <v>-0.92883617263419638</v>
+        <v>2.0892647180238755E-2</v>
       </c>
     </row>
     <row r="56" spans="4:14" x14ac:dyDescent="0.3">
@@ -3463,23 +3640,26 @@
       </c>
       <c r="E56">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515342</v>
+        <v>0.58778525229247425</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>-0.23176274578121103</v>
+        <v>-0.60676274578121003</v>
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
-        <v>0.29389262614623712</v>
+        <v>-0.47552825814757721</v>
       </c>
       <c r="H56">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747334</v>
+        <v>0.15450849718747245</v>
+      </c>
+      <c r="M56">
+        <v>5.4</v>
       </c>
       <c r="N56">
         <f>SUM(E56,F56,G56,H56)</f>
-        <v>-1.2934351331176006</v>
+        <v>-0.33999725444884055</v>
       </c>
     </row>
     <row r="57" spans="4:14" x14ac:dyDescent="0.3">
@@ -3488,23 +3668,26 @@
       </c>
       <c r="E57">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>4.9003769791999829E-15</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>-1.8376413671999936E-15</v>
+        <v>-0.75</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
-        <v>2.4501884895999915E-15</v>
+        <v>-4.9003769791999829E-15</v>
       </c>
       <c r="H57">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M57">
+        <v>5.5</v>
       </c>
       <c r="N57">
         <f>SUM(E57,F57,G57,H57)</f>
-        <v>-1.4999999999999993</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="58" spans="4:14" x14ac:dyDescent="0.3">
@@ -3513,23 +3696,26 @@
       </c>
       <c r="E58">
         <f t="shared" si="0"/>
-        <v>-0.95105651629515375</v>
+        <v>-0.58778525229247203</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>0.23176274578121009</v>
+        <v>-0.60676274578121114</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623601</v>
+        <v>0.47552825814757638</v>
       </c>
       <c r="H58">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747411</v>
+        <v>0.15450849718747503</v>
+      </c>
+      <c r="M58">
+        <v>5.6</v>
       </c>
       <c r="N58">
         <f>SUM(E58,F58,G58,H58)</f>
-        <v>-1.4176948938476539</v>
+        <v>-0.56451124273863185</v>
       </c>
     </row>
     <row r="59" spans="4:14" x14ac:dyDescent="0.3">
@@ -3538,23 +3724,26 @@
       </c>
       <c r="E59">
         <f t="shared" si="0"/>
-        <v>-0.80901699437494679</v>
+        <v>-0.9510565162951542</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
-        <v>0.44083893921935552</v>
+        <v>-0.23176274578120903</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
-        <v>-0.4755282581475771</v>
+        <v>0.29389262614623485</v>
       </c>
       <c r="H59">
         <f t="shared" si="3"/>
-        <v>-0.1545084971874727</v>
+        <v>-0.404508497187475</v>
+      </c>
+      <c r="M59">
+        <v>5.7</v>
       </c>
       <c r="N59">
         <f>SUM(E59,F59,G59,H59)</f>
-        <v>-0.99821481049064109</v>
+        <v>-1.2934351331176033</v>
       </c>
     </row>
     <row r="60" spans="4:14" x14ac:dyDescent="0.3">
@@ -3563,23 +3752,26 @@
       </c>
       <c r="E60">
         <f t="shared" si="0"/>
-        <v>-0.58778525229247369</v>
+        <v>-0.95105651629515398</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>0.60676274578121026</v>
+        <v>0.23176274578120953</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>-0.47552825814757699</v>
+        <v>-0.2938926261462354</v>
       </c>
       <c r="H60">
         <f t="shared" si="3"/>
-        <v>0.15450849718747303</v>
+        <v>-0.40450849718747456</v>
+      </c>
+      <c r="M60">
+        <v>5.8</v>
       </c>
       <c r="N60">
         <f>SUM(E60,F60,G60,H60)</f>
-        <v>-0.30204226747136742</v>
+        <v>-1.4176948938476543</v>
       </c>
     </row>
     <row r="61" spans="4:14" x14ac:dyDescent="0.3">
@@ -3588,23 +3780,26 @@
       </c>
       <c r="E61">
         <f t="shared" si="0"/>
-        <v>-0.3090169943749464</v>
+        <v>-0.58778525229247147</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>0.71329238722136545</v>
+        <v>0.60676274578121148</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
-        <v>-0.29389262614623574</v>
+        <v>-0.47552825814757615</v>
       </c>
       <c r="H61">
         <f t="shared" si="3"/>
-        <v>0.40450849718747434</v>
+        <v>0.15450849718747572</v>
+      </c>
+      <c r="M61">
+        <v>5.9</v>
       </c>
       <c r="N61">
         <f>SUM(E61,F61,G61,H61)</f>
-        <v>0.51489126388765771</v>
+        <v>-0.30204226747136043</v>
       </c>
     </row>
     <row r="62" spans="4:14" x14ac:dyDescent="0.3">
@@ -3613,7 +3808,7 @@
       </c>
       <c r="E62">
         <f t="shared" si="0"/>
-        <v>-7.3508907294517201E-16</v>
+        <v>-1.470178145890344E-15</v>
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
@@ -3621,15 +3816,18 @@
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
-        <v>-7.3508907294517201E-16</v>
+        <v>-1.470178145890344E-15</v>
       </c>
       <c r="H62">
         <f t="shared" si="3"/>
         <v>0.5</v>
+      </c>
+      <c r="M62">
+        <v>6</v>
       </c>
       <c r="N62">
         <f>SUM(E62,F62,G62,H62)</f>
-        <v>1.2499999999999984</v>
+        <v>1.2499999999999971</v>
       </c>
     </row>
     <row r="63" spans="4:14" x14ac:dyDescent="0.3">
@@ -3638,23 +3836,26 @@
       </c>
       <c r="E63">
         <f t="shared" si="0"/>
-        <v>0.30901699437494501</v>
+        <v>0.58778525229246903</v>
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>0.71329238722136568</v>
+        <v>0.60676274578121281</v>
       </c>
       <c r="G63">
         <f t="shared" si="2"/>
-        <v>0.29389262614623451</v>
+        <v>0.47552825814757521</v>
       </c>
       <c r="H63">
         <f t="shared" si="3"/>
-        <v>0.40450849718747517</v>
+        <v>0.1545084971874785</v>
+      </c>
+      <c r="M63">
+        <v>6.1</v>
       </c>
       <c r="N63">
         <f>SUM(E63,F63,G63,H63)</f>
-        <v>1.7207105049300204</v>
+        <v>1.8245847534087356</v>
       </c>
     </row>
     <row r="64" spans="4:14" x14ac:dyDescent="0.3">
@@ -3663,23 +3864,26 @@
       </c>
       <c r="E64">
         <f t="shared" si="0"/>
-        <v>0.58778525229247247</v>
+        <v>0.95105651629515309</v>
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>0.60676274578121092</v>
+        <v>0.23176274578121167</v>
       </c>
       <c r="G64">
         <f t="shared" si="2"/>
-        <v>0.47552825814757654</v>
+        <v>0.29389262614623779</v>
       </c>
       <c r="H64">
         <f t="shared" si="3"/>
-        <v>0.15450849718747445</v>
+        <v>-0.40450849718747284</v>
+      </c>
+      <c r="M64">
+        <v>6.2</v>
       </c>
       <c r="N64">
         <f>SUM(E64,F64,G64,H64)</f>
-        <v>1.8245847534087343</v>
+        <v>1.0722033910351296</v>
       </c>
     </row>
     <row r="65" spans="4:14" x14ac:dyDescent="0.3">
@@ -3688,23 +3892,26 @@
       </c>
       <c r="E65">
         <f t="shared" si="0"/>
-        <v>0.8090169943749459</v>
+        <v>0.9510565162951552</v>
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>0.44083893921935635</v>
+        <v>-0.23176274578120692</v>
       </c>
       <c r="G65">
         <f t="shared" si="2"/>
-        <v>0.4755282581475776</v>
+        <v>-0.29389262614623246</v>
       </c>
       <c r="H65">
         <f t="shared" si="3"/>
-        <v>-0.15450849718747128</v>
+        <v>-0.40450849718747672</v>
+      </c>
+      <c r="M65">
+        <v>6.3</v>
       </c>
       <c r="N65">
         <f>SUM(E65,F65,G65,H65)</f>
-        <v>1.5708756945544085</v>
+        <v>2.0892647180239088E-2</v>
       </c>
     </row>
     <row r="66" spans="4:14" x14ac:dyDescent="0.3">
@@ -3713,23 +3920,26 @@
       </c>
       <c r="E66">
         <f t="shared" si="0"/>
-        <v>0.95105651629515331</v>
+        <v>0.58778525229247436</v>
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>0.23176274578121114</v>
+        <v>-0.60676274578120981</v>
       </c>
       <c r="G66">
         <f t="shared" si="2"/>
-        <v>0.29389262614623718</v>
+        <v>-0.47552825814757727</v>
       </c>
       <c r="H66">
         <f t="shared" si="3"/>
-        <v>-0.40450849718747323</v>
+        <v>0.15450849718747223</v>
+      </c>
+      <c r="M66">
+        <v>6.4</v>
       </c>
       <c r="N66">
         <f>SUM(E66,F66,G66,H66)</f>
-        <v>1.0722033910351283</v>
+        <v>-0.33999725444884049</v>
       </c>
     </row>
     <row r="67" spans="4:14" x14ac:dyDescent="0.3">
@@ -3737,24 +3947,27 @@
         <v>6.5</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E102" si="4">B$3*SIN(B$2*PI()*D67)</f>
-        <v>1</v>
+        <f t="shared" ref="E67:E102" si="4">B$3*SIN(B$2*2*PI()*D67)</f>
+        <v>-1.9600206874192949E-15</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F102" si="5">B$4*COS(B$2*PI()*D67)</f>
-        <v>-7.3500775778223559E-16</v>
+        <f t="shared" ref="F67:F102" si="5">B$4*COS(B$2*2*PI()*D67)</f>
+        <v>-0.75</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G102" si="6">B$5*SIN(2*B$2*PI()*D67)</f>
-        <v>-9.8001034370964746E-16</v>
+        <f t="shared" ref="G67:G102" si="6">B$5*SIN(2*B$2*2*PI()*D67)</f>
+        <v>1.9600206874192949E-15</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H102" si="7">B$5*COS(2*B$2*PI()*D67)</f>
-        <v>-0.5</v>
+        <f t="shared" ref="H67:H102" si="7">B$5*COS(2*B$2*2*PI()*D67)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M67">
+        <v>6.5</v>
       </c>
       <c r="N67">
         <f>SUM(E67,F67,G67,H67)</f>
-        <v>0.49999999999999822</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="68" spans="4:14" x14ac:dyDescent="0.3">
@@ -3763,23 +3976,26 @@
       </c>
       <c r="E68">
         <f t="shared" si="4"/>
-        <v>0.95105651629515386</v>
+        <v>-0.5877852522924718</v>
       </c>
       <c r="F68">
         <f t="shared" si="5"/>
-        <v>-0.23176274578121001</v>
+        <v>-0.60676274578121125</v>
       </c>
       <c r="G68">
         <f t="shared" si="6"/>
-        <v>-0.2938926261462359</v>
+        <v>0.47552825814757627</v>
       </c>
       <c r="H68">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747417</v>
+        <v>0.15450849718747525</v>
+      </c>
+      <c r="M68">
+        <v>6.6</v>
       </c>
       <c r="N68">
         <f>SUM(E68,F68,G68,H68)</f>
-        <v>2.0892647180233759E-2</v>
+        <v>-0.56451124273863151</v>
       </c>
     </row>
     <row r="69" spans="4:14" x14ac:dyDescent="0.3">
@@ -3788,23 +4004,26 @@
       </c>
       <c r="E69">
         <f t="shared" si="4"/>
-        <v>0.8090169943749469</v>
+        <v>-0.9510565162951542</v>
       </c>
       <c r="F69">
         <f t="shared" si="5"/>
-        <v>-0.44083893921935546</v>
+        <v>-0.2317627457812092</v>
       </c>
       <c r="G69">
         <f t="shared" si="6"/>
-        <v>-0.4755282581475771</v>
+        <v>0.29389262614623501</v>
       </c>
       <c r="H69">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747281</v>
+        <v>-0.40450849718747484</v>
+      </c>
+      <c r="M69">
+        <v>6.7</v>
       </c>
       <c r="N69">
         <f>SUM(E69,F69,G69,H69)</f>
-        <v>-0.26185870017945845</v>
+        <v>-1.2934351331176033</v>
       </c>
     </row>
     <row r="70" spans="4:14" x14ac:dyDescent="0.3">
@@ -3813,23 +4032,26 @@
       </c>
       <c r="E70">
         <f t="shared" si="4"/>
-        <v>0.5877852522924738</v>
+        <v>-0.95105651629515409</v>
       </c>
       <c r="F70">
         <f t="shared" si="5"/>
-        <v>-0.60676274578121014</v>
+        <v>0.23176274578120937</v>
       </c>
       <c r="G70">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757704</v>
+        <v>-0.29389262614623524</v>
       </c>
       <c r="H70">
         <f t="shared" si="7"/>
-        <v>0.15450849718747292</v>
+        <v>-0.40450849718747467</v>
+      </c>
+      <c r="M70">
+        <v>6.8</v>
       </c>
       <c r="N70">
         <f>SUM(E70,F70,G70,H70)</f>
-        <v>-0.33999725444884044</v>
+        <v>-1.4176948938476546</v>
       </c>
     </row>
     <row r="71" spans="4:14" x14ac:dyDescent="0.3">
@@ -3838,23 +4060,26 @@
       </c>
       <c r="E71">
         <f t="shared" si="4"/>
-        <v>0.30901699437494656</v>
+        <v>-0.58778525229247158</v>
       </c>
       <c r="F71">
         <f t="shared" si="5"/>
-        <v>-0.71329238722136545</v>
+        <v>0.60676274578121148</v>
       </c>
       <c r="G71">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623579</v>
+        <v>-0.47552825814757621</v>
       </c>
       <c r="H71">
         <f t="shared" si="7"/>
-        <v>0.40450849718747428</v>
+        <v>0.15450849718747547</v>
+      </c>
+      <c r="M71">
+        <v>6.9</v>
       </c>
       <c r="N71">
         <f>SUM(E71,F71,G71,H71)</f>
-        <v>-0.2936595218051804</v>
+        <v>-0.30204226747136087</v>
       </c>
     </row>
     <row r="72" spans="4:14" x14ac:dyDescent="0.3">
@@ -3863,23 +4088,26 @@
       </c>
       <c r="E72">
         <f t="shared" si="4"/>
-        <v>8.5760391843603401E-16</v>
+        <v>-1.715207836872068E-15</v>
       </c>
       <c r="F72">
         <f t="shared" si="5"/>
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G72">
         <f t="shared" si="6"/>
-        <v>-8.5760391843603401E-16</v>
+        <v>-1.715207836872068E-15</v>
       </c>
       <c r="H72">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
+      <c r="M72">
+        <v>7</v>
+      </c>
       <c r="N72">
         <f>SUM(E72,F72,G72,H72)</f>
-        <v>-0.25</v>
+        <v>1.2499999999999967</v>
       </c>
     </row>
     <row r="73" spans="4:14" x14ac:dyDescent="0.3">
@@ -3888,23 +4116,26 @@
       </c>
       <c r="E73">
         <f t="shared" si="4"/>
-        <v>-0.3090169943749449</v>
+        <v>0.58778525229246881</v>
       </c>
       <c r="F73">
         <f t="shared" si="5"/>
-        <v>-0.71329238722136579</v>
+        <v>0.60676274578121292</v>
       </c>
       <c r="G73">
         <f t="shared" si="6"/>
-        <v>0.2938926261462344</v>
+        <v>0.47552825814757516</v>
       </c>
       <c r="H73">
         <f t="shared" si="7"/>
-        <v>0.40450849718747528</v>
+        <v>0.15450849718747875</v>
+      </c>
+      <c r="M73">
+        <v>7.1</v>
       </c>
       <c r="N73">
         <f>SUM(E73,F73,G73,H73)</f>
-        <v>-0.32390825826260095</v>
+        <v>1.8245847534087358</v>
       </c>
     </row>
     <row r="74" spans="4:14" x14ac:dyDescent="0.3">
@@ -3913,23 +4144,26 @@
       </c>
       <c r="E74">
         <f t="shared" si="4"/>
-        <v>-0.58778525229247247</v>
+        <v>0.95105651629515298</v>
       </c>
       <c r="F74">
         <f t="shared" si="5"/>
-        <v>-0.60676274578121092</v>
+        <v>0.23176274578121184</v>
       </c>
       <c r="G74">
         <f t="shared" si="6"/>
-        <v>0.47552825814757649</v>
+        <v>0.29389262614623801</v>
       </c>
       <c r="H74">
         <f t="shared" si="7"/>
-        <v>0.15450849718747456</v>
+        <v>-0.40450849718747267</v>
+      </c>
+      <c r="M74">
+        <v>7.2</v>
       </c>
       <c r="N74">
         <f>SUM(E74,F74,G74,H74)</f>
-        <v>-0.56451124273863229</v>
+        <v>1.0722033910351303</v>
       </c>
     </row>
     <row r="75" spans="4:14" x14ac:dyDescent="0.3">
@@ -3938,23 +4172,26 @@
       </c>
       <c r="E75">
         <f t="shared" si="4"/>
-        <v>-0.8090169943749459</v>
+        <v>0.9510565162951552</v>
       </c>
       <c r="F75">
         <f t="shared" si="5"/>
-        <v>-0.44083893921935646</v>
+        <v>-0.23176274578120676</v>
       </c>
       <c r="G75">
         <f t="shared" si="6"/>
-        <v>0.4755282581475776</v>
+        <v>-0.29389262614623224</v>
       </c>
       <c r="H75">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747117</v>
+        <v>-0.40450849718747683</v>
+      </c>
+      <c r="M75">
+        <v>7.3</v>
       </c>
       <c r="N75">
         <f>SUM(E75,F75,G75,H75)</f>
-        <v>-0.92883617263419604</v>
+        <v>2.089264718023931E-2</v>
       </c>
     </row>
     <row r="76" spans="4:14" x14ac:dyDescent="0.3">
@@ -3963,23 +4200,26 @@
       </c>
       <c r="E76">
         <f t="shared" si="4"/>
-        <v>-0.95105651629515331</v>
+        <v>0.58778525229247458</v>
       </c>
       <c r="F76">
         <f t="shared" si="5"/>
-        <v>-0.2317627457812112</v>
+        <v>-0.6067627457812097</v>
       </c>
       <c r="G76">
         <f t="shared" si="6"/>
-        <v>0.29389262614623729</v>
+        <v>-0.47552825814757732</v>
       </c>
       <c r="H76">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747317</v>
+        <v>0.15450849718747198</v>
+      </c>
+      <c r="M76">
+        <v>7.4</v>
       </c>
       <c r="N76">
         <f>SUM(E76,F76,G76,H76)</f>
-        <v>-1.2934351331176002</v>
+        <v>-0.33999725444884044</v>
       </c>
     </row>
     <row r="77" spans="4:14" x14ac:dyDescent="0.3">
@@ -3988,23 +4228,26 @@
       </c>
       <c r="E77">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>5.3904363611634309E-15</v>
       </c>
       <c r="F77">
         <f t="shared" si="5"/>
-        <v>-2.0214136354362866E-15</v>
+        <v>-0.75</v>
       </c>
       <c r="G77">
         <f t="shared" si="6"/>
-        <v>2.6952181805817155E-15</v>
+        <v>-5.3904363611634309E-15</v>
       </c>
       <c r="H77">
         <f t="shared" si="7"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M77">
+        <v>7.5</v>
       </c>
       <c r="N77">
         <f>SUM(E77,F77,G77,H77)</f>
-        <v>-1.4999999999999993</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="78" spans="4:14" x14ac:dyDescent="0.3">
@@ -4013,23 +4256,26 @@
       </c>
       <c r="E78">
         <f t="shared" si="4"/>
-        <v>-0.95105651629515386</v>
+        <v>-0.58778525229247158</v>
       </c>
       <c r="F78">
         <f t="shared" si="5"/>
-        <v>0.23176274578120992</v>
+        <v>-0.60676274578121148</v>
       </c>
       <c r="G78">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623579</v>
+        <v>0.47552825814757621</v>
       </c>
       <c r="H78">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747428</v>
+        <v>0.15450849718747547</v>
+      </c>
+      <c r="M78">
+        <v>7.6</v>
       </c>
       <c r="N78">
         <f>SUM(E78,F78,G78,H78)</f>
-        <v>-1.4176948938476541</v>
+        <v>-0.5645112427386314</v>
       </c>
     </row>
     <row r="79" spans="4:14" x14ac:dyDescent="0.3">
@@ -4038,23 +4284,26 @@
       </c>
       <c r="E79">
         <f t="shared" si="4"/>
-        <v>-0.8090169943749469</v>
+        <v>-0.95105651629515409</v>
       </c>
       <c r="F79">
         <f t="shared" si="5"/>
-        <v>0.44083893921935535</v>
+        <v>-0.23176274578120937</v>
       </c>
       <c r="G79">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757704</v>
+        <v>0.29389262614623524</v>
       </c>
       <c r="H79">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747292</v>
+        <v>-0.40450849718747467</v>
+      </c>
+      <c r="M79">
+        <v>7.7</v>
       </c>
       <c r="N79">
         <f>SUM(E79,F79,G79,H79)</f>
-        <v>-0.99821481049064154</v>
+        <v>-1.2934351331176031</v>
       </c>
     </row>
     <row r="80" spans="4:14" x14ac:dyDescent="0.3">
@@ -4063,23 +4312,26 @@
       </c>
       <c r="E80">
         <f t="shared" si="4"/>
-        <v>-0.58778525229247391</v>
+        <v>-0.9510565162951542</v>
       </c>
       <c r="F80">
         <f t="shared" si="5"/>
-        <v>0.60676274578121014</v>
+        <v>0.2317627457812092</v>
       </c>
       <c r="G80">
         <f t="shared" si="6"/>
-        <v>-0.4755282581475771</v>
+        <v>-0.29389262614623501</v>
       </c>
       <c r="H80">
         <f t="shared" si="7"/>
-        <v>0.15450849718747281</v>
+        <v>-0.40450849718747484</v>
+      </c>
+      <c r="M80">
+        <v>7.8</v>
       </c>
       <c r="N80">
         <f>SUM(E80,F80,G80,H80)</f>
-        <v>-0.30204226747136809</v>
+        <v>-1.4176948938476548</v>
       </c>
     </row>
     <row r="81" spans="4:14" x14ac:dyDescent="0.3">
@@ -4088,23 +4340,26 @@
       </c>
       <c r="E81">
         <f t="shared" si="4"/>
-        <v>-0.30901699437494667</v>
+        <v>-0.5877852522924718</v>
       </c>
       <c r="F81">
         <f t="shared" si="5"/>
-        <v>0.71329238722136545</v>
+        <v>0.60676274578121125</v>
       </c>
       <c r="G81">
         <f t="shared" si="6"/>
-        <v>-0.2938926261462359</v>
+        <v>-0.47552825814757627</v>
       </c>
       <c r="H81">
         <f t="shared" si="7"/>
-        <v>0.40450849718747417</v>
+        <v>0.15450849718747525</v>
+      </c>
+      <c r="M81">
+        <v>7.9</v>
       </c>
       <c r="N81">
         <f>SUM(E81,F81,G81,H81)</f>
-        <v>0.51489126388765705</v>
+        <v>-0.30204226747136154</v>
       </c>
     </row>
     <row r="82" spans="4:14" x14ac:dyDescent="0.3">
@@ -4113,7 +4368,7 @@
       </c>
       <c r="E82">
         <f t="shared" si="4"/>
-        <v>-9.8011876392689601E-16</v>
+        <v>-1.960237527853792E-15</v>
       </c>
       <c r="F82">
         <f t="shared" si="5"/>
@@ -4121,15 +4376,18 @@
       </c>
       <c r="G82">
         <f t="shared" si="6"/>
-        <v>-9.8011876392689601E-16</v>
+        <v>-1.960237527853792E-15</v>
       </c>
       <c r="H82">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
+      <c r="M82">
+        <v>8</v>
+      </c>
       <c r="N82">
         <f>SUM(E82,F82,G82,H82)</f>
-        <v>1.249999999999998</v>
+        <v>1.249999999999996</v>
       </c>
     </row>
     <row r="83" spans="4:14" x14ac:dyDescent="0.3">
@@ -4138,23 +4396,26 @@
       </c>
       <c r="E83">
         <f t="shared" si="4"/>
-        <v>0.30901699437494479</v>
+        <v>0.5877852522924687</v>
       </c>
       <c r="F83">
         <f t="shared" si="5"/>
-        <v>0.71329238722136579</v>
+        <v>0.60676274578121303</v>
       </c>
       <c r="G83">
         <f t="shared" si="6"/>
-        <v>0.29389262614623435</v>
+        <v>0.4755282581475751</v>
       </c>
       <c r="H83">
         <f t="shared" si="7"/>
-        <v>0.40450849718747534</v>
+        <v>0.15450849718747897</v>
+      </c>
+      <c r="M83">
+        <v>8.1</v>
       </c>
       <c r="N83">
         <f>SUM(E83,F83,G83,H83)</f>
-        <v>1.7207105049300202</v>
+        <v>1.8245847534087358</v>
       </c>
     </row>
     <row r="84" spans="4:14" x14ac:dyDescent="0.3">
@@ -4163,23 +4424,26 @@
       </c>
       <c r="E84">
         <f t="shared" si="4"/>
-        <v>0.58778525229246947</v>
+        <v>0.95105651629515076</v>
       </c>
       <c r="F84">
         <f t="shared" si="5"/>
-        <v>0.60676274578121259</v>
+        <v>0.23176274578121708</v>
       </c>
       <c r="G84">
         <f t="shared" si="6"/>
-        <v>0.47552825814757538</v>
+        <v>0.29389262614624395</v>
       </c>
       <c r="H84">
         <f t="shared" si="7"/>
-        <v>0.15450849718747806</v>
+        <v>-0.40450849718746834</v>
+      </c>
+      <c r="M84">
+        <v>8.1999999999999993</v>
       </c>
       <c r="N84">
         <f>SUM(E84,F84,G84,H84)</f>
-        <v>1.8245847534087356</v>
+        <v>1.0722033910351434</v>
       </c>
     </row>
     <row r="85" spans="4:14" x14ac:dyDescent="0.3">
@@ -4188,23 +4452,26 @@
       </c>
       <c r="E85">
         <f t="shared" si="4"/>
-        <v>0.8090169943749479</v>
+        <v>0.95105651629515309</v>
       </c>
       <c r="F85">
         <f t="shared" si="5"/>
-        <v>0.44083893921935435</v>
+        <v>-0.23176274578121167</v>
       </c>
       <c r="G85">
         <f t="shared" si="6"/>
-        <v>0.47552825814757654</v>
+        <v>-0.29389262614623779</v>
       </c>
       <c r="H85">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747445</v>
+        <v>-0.40450849718747284</v>
+      </c>
+      <c r="M85">
+        <v>8.3000000000000007</v>
       </c>
       <c r="N85">
         <f>SUM(E85,F85,G85,H85)</f>
-        <v>1.5708756945544045</v>
+        <v>2.0892647180230761E-2</v>
       </c>
     </row>
     <row r="86" spans="4:14" x14ac:dyDescent="0.3">
@@ -4213,23 +4480,26 @@
       </c>
       <c r="E86">
         <f t="shared" si="4"/>
-        <v>0.95105651629515331</v>
+        <v>0.5877852522924748</v>
       </c>
       <c r="F86">
         <f t="shared" si="5"/>
-        <v>0.23176274578121131</v>
+        <v>-0.6067627457812097</v>
       </c>
       <c r="G86">
         <f t="shared" si="6"/>
-        <v>0.2938926261462374</v>
+        <v>-0.47552825814757743</v>
       </c>
       <c r="H86">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747312</v>
+        <v>0.15450849718747175</v>
+      </c>
+      <c r="M86">
+        <v>8.4</v>
       </c>
       <c r="N86">
         <f>SUM(E86,F86,G86,H86)</f>
-        <v>1.072203391035129</v>
+        <v>-0.33999725444884055</v>
       </c>
     </row>
     <row r="87" spans="4:14" x14ac:dyDescent="0.3">
@@ -4238,23 +4508,26 @@
       </c>
       <c r="E87">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-1.4699613054558469E-15</v>
       </c>
       <c r="F87">
         <f t="shared" si="5"/>
-        <v>-5.5123548954594259E-16</v>
+        <v>-0.75</v>
       </c>
       <c r="G87">
         <f t="shared" si="6"/>
-        <v>-7.3498065272792346E-16</v>
+        <v>1.4699613054558469E-15</v>
       </c>
       <c r="H87">
         <f t="shared" si="7"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M87">
+        <v>8.5</v>
       </c>
       <c r="N87">
         <f>SUM(E87,F87,G87,H87)</f>
-        <v>0.49999999999999867</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="88" spans="4:14" x14ac:dyDescent="0.3">
@@ -4263,23 +4536,26 @@
       </c>
       <c r="E88">
         <f t="shared" si="4"/>
-        <v>0.95105651629515386</v>
+        <v>-0.58778525229247147</v>
       </c>
       <c r="F88">
         <f t="shared" si="5"/>
-        <v>-0.23176274578120981</v>
+        <v>-0.60676274578121148</v>
       </c>
       <c r="G88">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623574</v>
+        <v>0.47552825814757615</v>
       </c>
       <c r="H88">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747434</v>
+        <v>0.15450849718747572</v>
+      </c>
+      <c r="M88">
+        <v>8.6</v>
       </c>
       <c r="N88">
         <f>SUM(E88,F88,G88,H88)</f>
-        <v>2.0892647180233981E-2</v>
+        <v>-0.56451124273863096</v>
       </c>
     </row>
     <row r="89" spans="4:14" x14ac:dyDescent="0.3">
@@ -4288,23 +4564,26 @@
       </c>
       <c r="E89">
         <f t="shared" si="4"/>
-        <v>0.80901699437494912</v>
+        <v>-0.95105651629515187</v>
       </c>
       <c r="F89">
         <f t="shared" si="5"/>
-        <v>-0.44083893921935313</v>
+        <v>-0.23176274578121464</v>
       </c>
       <c r="G89">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757593</v>
+        <v>0.29389262614624118</v>
       </c>
       <c r="H89">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747642</v>
+        <v>-0.40450849718747039</v>
+      </c>
+      <c r="M89">
+        <v>8.6999999999999993</v>
       </c>
       <c r="N89">
         <f>SUM(E89,F89,G89,H89)</f>
-        <v>-0.26185870017945634</v>
+        <v>-1.2934351331175957</v>
       </c>
     </row>
     <row r="90" spans="4:14" x14ac:dyDescent="0.3">
@@ -4313,23 +4592,26 @@
       </c>
       <c r="E90">
         <f t="shared" si="4"/>
-        <v>0.58778525229247114</v>
+        <v>-0.95105651629515209</v>
       </c>
       <c r="F90">
         <f t="shared" si="5"/>
-        <v>-0.6067627457812117</v>
+        <v>0.23176274578121409</v>
       </c>
       <c r="G90">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757604</v>
+        <v>-0.29389262614624057</v>
       </c>
       <c r="H90">
         <f t="shared" si="7"/>
-        <v>0.15450849718747606</v>
+        <v>-0.40450849718747078</v>
+      </c>
+      <c r="M90">
+        <v>8.8000000000000007</v>
       </c>
       <c r="N90">
         <f>SUM(E90,F90,G90,H90)</f>
-        <v>-0.33999725444884055</v>
+        <v>-1.4176948938476495</v>
       </c>
     </row>
     <row r="91" spans="4:14" x14ac:dyDescent="0.3">
@@ -4338,23 +4620,26 @@
       </c>
       <c r="E91">
         <f t="shared" si="4"/>
-        <v>0.30901699437494679</v>
+        <v>-0.58778525229247203</v>
       </c>
       <c r="F91">
         <f t="shared" si="5"/>
-        <v>-0.71329238722136534</v>
+        <v>0.60676274578121114</v>
       </c>
       <c r="G91">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623601</v>
+        <v>-0.47552825814757638</v>
       </c>
       <c r="H91">
         <f t="shared" si="7"/>
-        <v>0.40450849718747411</v>
+        <v>0.15450849718747503</v>
+      </c>
+      <c r="M91">
+        <v>8.9</v>
       </c>
       <c r="N91">
         <f>SUM(E91,F91,G91,H91)</f>
-        <v>-0.29365952180518046</v>
+        <v>-0.3020422674713622</v>
       </c>
     </row>
     <row r="92" spans="4:14" x14ac:dyDescent="0.3">
@@ -4363,23 +4648,26 @@
       </c>
       <c r="E92">
         <f t="shared" si="4"/>
-        <v>1.102633609417758E-15</v>
+        <v>-2.205267218835516E-15</v>
       </c>
       <c r="F92">
         <f t="shared" si="5"/>
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G92">
         <f t="shared" si="6"/>
-        <v>-1.102633609417758E-15</v>
+        <v>-2.205267218835516E-15</v>
       </c>
       <c r="H92">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
+      <c r="M92">
+        <v>9</v>
+      </c>
       <c r="N92">
         <f>SUM(E92,F92,G92,H92)</f>
-        <v>-0.25</v>
+        <v>1.2499999999999956</v>
       </c>
     </row>
     <row r="93" spans="4:14" x14ac:dyDescent="0.3">
@@ -4388,23 +4676,26 @@
       </c>
       <c r="E93">
         <f t="shared" si="4"/>
-        <v>-0.30901699437494468</v>
+        <v>0.58778525229246847</v>
       </c>
       <c r="F93">
         <f t="shared" si="5"/>
-        <v>-0.71329238722136579</v>
+        <v>0.60676274578121303</v>
       </c>
       <c r="G93">
         <f t="shared" si="6"/>
-        <v>0.29389262614623424</v>
+        <v>0.47552825814757499</v>
       </c>
       <c r="H93">
         <f t="shared" si="7"/>
-        <v>0.40450849718747539</v>
+        <v>0.15450849718747922</v>
+      </c>
+      <c r="M93">
+        <v>9.1</v>
       </c>
       <c r="N93">
         <f>SUM(E93,F93,G93,H93)</f>
-        <v>-0.32390825826260083</v>
+        <v>1.8245847534087358</v>
       </c>
     </row>
     <row r="94" spans="4:14" x14ac:dyDescent="0.3">
@@ -4413,23 +4704,26 @@
       </c>
       <c r="E94">
         <f t="shared" si="4"/>
-        <v>-0.58778525229246936</v>
+        <v>0.95105651629515064</v>
       </c>
       <c r="F94">
         <f t="shared" si="5"/>
-        <v>-0.6067627457812127</v>
+        <v>0.23176274578121725</v>
       </c>
       <c r="G94">
         <f t="shared" si="6"/>
-        <v>0.47552825814757532</v>
+        <v>0.29389262614624412</v>
       </c>
       <c r="H94">
         <f t="shared" si="7"/>
-        <v>0.15450849718747817</v>
+        <v>-0.40450849718746823</v>
+      </c>
+      <c r="M94">
+        <v>9.1999999999999993</v>
       </c>
       <c r="N94">
         <f>SUM(E94,F94,G94,H94)</f>
-        <v>-0.56451124273862852</v>
+        <v>1.0722033910351441</v>
       </c>
     </row>
     <row r="95" spans="4:14" x14ac:dyDescent="0.3">
@@ -4438,23 +4732,26 @@
       </c>
       <c r="E95">
         <f t="shared" si="4"/>
-        <v>-0.80901699437494778</v>
+        <v>0.9510565162951532</v>
       </c>
       <c r="F95">
         <f t="shared" si="5"/>
-        <v>-0.44083893921935446</v>
+        <v>-0.23176274578121148</v>
       </c>
       <c r="G95">
         <f t="shared" si="6"/>
-        <v>0.4755282581475766</v>
+        <v>-0.29389262614623757</v>
       </c>
       <c r="H95">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747431</v>
+        <v>-0.40450849718747295</v>
+      </c>
+      <c r="M95">
+        <v>9.3000000000000007</v>
       </c>
       <c r="N95">
         <f>SUM(E95,F95,G95,H95)</f>
-        <v>-0.92883617263419993</v>
+        <v>2.0892647180231205E-2</v>
       </c>
     </row>
     <row r="96" spans="4:14" x14ac:dyDescent="0.3">
@@ -4463,23 +4760,26 @@
       </c>
       <c r="E96">
         <f t="shared" si="4"/>
-        <v>-0.9510565162951532</v>
+        <v>0.58778525229247502</v>
       </c>
       <c r="F96">
         <f t="shared" si="5"/>
-        <v>-0.23176274578121137</v>
+        <v>-0.60676274578120959</v>
       </c>
       <c r="G96">
         <f t="shared" si="6"/>
-        <v>0.29389262614623751</v>
+        <v>-0.47552825814757749</v>
       </c>
       <c r="H96">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747306</v>
+        <v>0.15450849718747153</v>
+      </c>
+      <c r="M96">
+        <v>9.4</v>
       </c>
       <c r="N96">
         <f>SUM(E96,F96,G96,H96)</f>
-        <v>-1.2934351331175999</v>
+        <v>-0.33999725444884055</v>
       </c>
     </row>
     <row r="97" spans="4:14" x14ac:dyDescent="0.3">
@@ -4488,23 +4788,26 @@
       </c>
       <c r="E97">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>5.8804957431268789E-15</v>
       </c>
       <c r="F97">
         <f t="shared" si="5"/>
-        <v>-2.2051859036725796E-15</v>
+        <v>-0.75</v>
       </c>
       <c r="G97">
         <f t="shared" si="6"/>
-        <v>2.9402478715634395E-15</v>
+        <v>-5.8804957431268789E-15</v>
       </c>
       <c r="H97">
         <f t="shared" si="7"/>
-        <v>-0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="M97">
+        <v>9.5</v>
       </c>
       <c r="N97">
         <f>SUM(E97,F97,G97,H97)</f>
-        <v>-1.4999999999999993</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="98" spans="4:14" x14ac:dyDescent="0.3">
@@ -4513,23 +4816,26 @@
       </c>
       <c r="E98">
         <f t="shared" si="4"/>
-        <v>-0.95105651629515398</v>
+        <v>-0.58778525229247125</v>
       </c>
       <c r="F98">
         <f t="shared" si="5"/>
-        <v>0.2317627457812097</v>
+        <v>-0.60676274578121159</v>
       </c>
       <c r="G98">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623562</v>
+        <v>0.47552825814757604</v>
       </c>
       <c r="H98">
         <f t="shared" si="7"/>
-        <v>-0.40450849718747439</v>
+        <v>0.15450849718747595</v>
+      </c>
+      <c r="M98">
+        <v>9.6</v>
       </c>
       <c r="N98">
         <f>SUM(E98,F98,G98,H98)</f>
-        <v>-1.4176948938476543</v>
+        <v>-0.56451124273863085</v>
       </c>
     </row>
     <row r="99" spans="4:14" x14ac:dyDescent="0.3">
@@ -4538,23 +4844,26 @@
       </c>
       <c r="E99">
         <f t="shared" si="4"/>
-        <v>-0.80901699437494912</v>
+        <v>-0.95105651629515175</v>
       </c>
       <c r="F99">
         <f t="shared" si="5"/>
-        <v>0.44083893921935302</v>
+        <v>-0.23176274578121481</v>
       </c>
       <c r="G99">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757588</v>
+        <v>0.29389262614624134</v>
       </c>
       <c r="H99">
         <f t="shared" si="7"/>
-        <v>-0.15450849718747653</v>
+        <v>-0.40450849718747023</v>
+      </c>
+      <c r="M99">
+        <v>9.6999999999999993</v>
       </c>
       <c r="N99">
         <f>SUM(E99,F99,G99,H99)</f>
-        <v>-0.99821481049064842</v>
+        <v>-1.2934351331175955</v>
       </c>
     </row>
     <row r="100" spans="4:14" x14ac:dyDescent="0.3">
@@ -4563,23 +4872,26 @@
       </c>
       <c r="E100">
         <f t="shared" si="4"/>
-        <v>-0.58778525229247125</v>
+        <v>-0.95105651629515209</v>
       </c>
       <c r="F100">
         <f t="shared" si="5"/>
-        <v>0.60676274578121159</v>
+        <v>0.23176274578121392</v>
       </c>
       <c r="G100">
         <f t="shared" si="6"/>
-        <v>-0.47552825814757604</v>
+        <v>-0.29389262614624034</v>
       </c>
       <c r="H100">
         <f t="shared" si="7"/>
-        <v>0.15450849718747595</v>
+        <v>-0.40450849718747095</v>
+      </c>
+      <c r="M100">
+        <v>9.8000000000000007</v>
       </c>
       <c r="N100">
         <f>SUM(E100,F100,G100,H100)</f>
-        <v>-0.30204226747135976</v>
+        <v>-1.4176948938476497</v>
       </c>
     </row>
     <row r="101" spans="4:14" x14ac:dyDescent="0.3">
@@ -4588,23 +4900,26 @@
       </c>
       <c r="E101">
         <f t="shared" si="4"/>
-        <v>-0.3090169943749469</v>
+        <v>-0.58778525229247225</v>
       </c>
       <c r="F101">
         <f t="shared" si="5"/>
-        <v>0.71329238722136534</v>
+        <v>0.60676274578121103</v>
       </c>
       <c r="G101">
         <f t="shared" si="6"/>
-        <v>-0.29389262614623612</v>
+        <v>-0.47552825814757643</v>
       </c>
       <c r="H101">
         <f t="shared" si="7"/>
-        <v>0.40450849718747406</v>
+        <v>0.15450849718747478</v>
+      </c>
+      <c r="M101">
+        <v>9.9</v>
       </c>
       <c r="N101">
         <f>SUM(E101,F101,G101,H101)</f>
-        <v>0.51489126388765638</v>
+        <v>-0.30204226747136287</v>
       </c>
     </row>
     <row r="102" spans="4:14" x14ac:dyDescent="0.3">
@@ -4613,7 +4928,7 @@
       </c>
       <c r="E102">
         <f t="shared" si="4"/>
-        <v>-1.22514845490862E-15</v>
+        <v>-2.45029690981724E-15</v>
       </c>
       <c r="F102">
         <f t="shared" si="5"/>
@@ -4621,15 +4936,18 @@
       </c>
       <c r="G102">
         <f t="shared" si="6"/>
-        <v>-1.22514845490862E-15</v>
+        <v>-2.45029690981724E-15</v>
       </c>
       <c r="H102">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
+      <c r="M102">
+        <v>10</v>
+      </c>
       <c r="N102">
         <f>SUM(E102,F102,G102,H102)</f>
-        <v>1.2499999999999976</v>
+        <v>1.2499999999999951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>